<commit_message>
New agenda for Cologne
</commit_message>
<xml_diff>
--- a/Agendas/201801 New Orleans WGM FHIR Agenda.xlsx
+++ b/Agendas/201801 New Orleans WGM FHIR Agenda.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="65">
   <si>
     <t>Mon</t>
   </si>
@@ -63,9 +63,6 @@
     <t>PHER</t>
   </si>
   <si>
-    <t>ITS</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>PC/CIMI/EC/Voc</t>
   </si>
   <si>
-    <t>InM/ITS</t>
-  </si>
-  <si>
     <t>Security/CBCC</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
   </si>
   <si>
     <t>Co-chairs dinner?</t>
-  </si>
-  <si>
-    <t>CBCC/Security</t>
   </si>
   <si>
     <t>Ref imps</t>
@@ -221,6 +212,12 @@
   </si>
   <si>
     <t>HSI?</t>
+  </si>
+  <si>
+    <t>CBCC</t>
+  </si>
+  <si>
+    <t>ITS</t>
   </si>
 </sst>
 </file>
@@ -282,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -300,6 +297,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -644,10 +644,10 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,22 +682,22 @@
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -705,16 +705,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -722,33 +722,33 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -756,19 +756,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -776,16 +776,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -793,33 +793,33 @@
         <v>2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,16 +827,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -844,50 +844,50 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -908,16 +908,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -925,33 +925,33 @@
         <v>2</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -960,16 +960,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -977,21 +977,21 @@
         <v>4</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1006,19 +1006,19 @@
         <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1026,36 +1026,36 @@
         <v>2</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1063,19 +1063,19 @@
         <v>3</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,16 +1083,16 @@
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,16 +1103,16 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1120,16 +1120,16 @@
         <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>47</v>
+        <v>16</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,16 +1143,16 @@
         <v>3</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1160,36 +1160,36 @@
         <v>4</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1197,16 +1197,16 @@
         <v>2</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1214,16 +1214,16 @@
         <v>3</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>